<commit_message>
add pdf modify test
</commit_message>
<xml_diff>
--- a/pcxzf/pcxzf/jiancefawenjian/网站监测反馈v3.0.xlsx
+++ b/pcxzf/pcxzf/jiancefawenjian/网站监测反馈v3.0.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,19 +442,19 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>一、法定主动公开内容栏目监测</t>
+          <t>五、基层政务公开专栏监测</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>检测时间：2024-10-21 10:30:39</t>
+          <t>检测时间：2025-02-14 17:50:39</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>1.栏目超期情况监测:以下位置栏目已超期，请责任部门更新</t>
+          <t>1.以下位置内容条数少于4条</t>
         </is>
       </c>
       <c r="B2" s="2" t="n"/>
@@ -463,66 +463,38 @@
       <c r="E2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>单位名称</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>领域</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>一级事项</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>二级事项</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>栏目更新检测标准</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="J4" t="inlineStr">
         <is>
           <t>栏目名称</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>更新标题</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>最后更新时间</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>超期天数</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>栏目更新检测标准</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>平昌县经济和信息化局</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>统计信息</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1-5月平昌县规上工业企业实现总产值                                            </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2024-06-20</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>123</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>栏目名称</t>
-        </is>
-      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>超期时间</t>
@@ -530,29 +502,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>平昌县财政局</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>其他法定信息</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">平昌县惠民惠农财政补贴资金“一卡通”政策汇编                                            </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2024-07-22</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>91</v>
-      </c>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2.以下位置最近更新时间大于330天</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
       <c r="J5" t="inlineStr">
         <is>
           <t>机关简介</t>
@@ -565,26 +523,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>平昌县交通运输局</t>
+          <t>单位名称</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>行政权力</t>
+          <t>领域</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">平昌县交通运输局行政许可事项受理公示                                            </t>
+          <t>一级事项</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>84</v>
+          <t>二级事项</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -598,26 +553,23 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>平昌县文化广播电视体育和旅游局</t>
+          <t>平昌县农业农村局</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>涉农补贴</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">平昌县文化广播电视体育和旅游局关于2023年度广播电视户户通运行维护资金绩效评价报告                                            </t>
+          <t>农业生产发展资金</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>81</v>
+          <t>农机购置补贴</t>
+        </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -631,26 +583,23 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>平昌县卫生健康局</t>
+          <t>平昌县农业农村局</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>涉农补贴</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">平昌县卫生健康局关于2023年部门整体支出绩效评价的报告                                            </t>
+          <t>农业生产发展资金</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>84</v>
+          <t>耕地地力保护</t>
+        </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -664,26 +613,23 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>平昌县审计局</t>
+          <t>平昌县农业农村局</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>涉农补贴</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">关于调整县委审计委员会组成人员的通知                                            </t>
+          <t>农业生产发展资金</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-17</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>96</v>
+          <t>种粮一次性补贴</t>
+        </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -697,26 +643,23 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>巴中市平昌生态环境局</t>
+          <t>平昌县农业农村局</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>预算/决算</t>
+          <t>涉农补贴</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">巴中市平昌生态环境局2022年度单位决算                                            </t>
+          <t>农业生产发展资金</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2023-10-13</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>374</v>
+          <t>稻谷补贴</t>
+        </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -730,26 +673,23 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>平昌县医疗保障局</t>
+          <t>平昌县市场监督管理局</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>统计信息</t>
+          <t>食品药品</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">2023年度平昌县医疗费用报费情况                                            </t>
+          <t>行政审批</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-06-07</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>136</v>
+          <t>食品生产经营许可基本信息</t>
+        </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -763,26 +703,23 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>平昌县行政审批和数据局</t>
+          <t>平昌县市场监督管理局</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>放管服改革</t>
+          <t>食品药品</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">【优化营商环境】白衣镇抓好并联审批落地提升政务服务水平                                            </t>
+          <t>监督检查</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2022-09-05</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>777</v>
+          <t>食品生产经营监督检查</t>
+        </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -796,26 +733,23 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>平昌县金宝新区管理委员会</t>
+          <t>平昌县市场监督管理局</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>统计信息</t>
+          <t>食品药品</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">金宝新区环境综合治理情况统计                                            </t>
+          <t>监督检查</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-25</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>88</v>
+          <t>由县级组织的医疗器械抽检</t>
+        </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -829,26 +763,23 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>平昌县金宝新区管理委员会</t>
+          <t>平昌县市场监督管理局</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>食品药品</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">金宝新区民政资金对象专项检查工作开展情况报告                                            </t>
+          <t>公共服务</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-25</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>88</v>
+          <t>食品用药安全宣传和消费提示警示</t>
+        </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -862,26 +793,23 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>平昌县金宝新区管理委员会</t>
+          <t>平昌县民政局</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>社会救助</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">金宝新区2024年扫黑除恶工作情况                                            </t>
+          <t>最低生活保障</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-25</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>88</v>
+          <t>政策法规文件</t>
+        </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -895,26 +823,23 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>平昌县白衣镇人民政府</t>
+          <t>平昌县教育科技局</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>统计信息</t>
+          <t>义务教育</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">平昌县白衣镇村居委会完整名称核实表                                            </t>
+          <t>教育概况</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-17</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>96</v>
+          <t>教育统计数据</t>
+        </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -928,26 +853,23 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>平昌县白衣镇人民政府</t>
+          <t>平昌县教育科技局</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>义务教育</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">2024年新增高龄人口                                            </t>
+          <t>学生管理</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-23</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>90</v>
+          <t>学生评优奖励</t>
+        </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -961,26 +883,23 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>平昌县白衣镇人民政府</t>
+          <t>平昌县教育科技局</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>义务教育</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">白衣镇2024年艾滋病防治工作实施方案                                            </t>
+          <t>教师管理</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-22</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>91</v>
+          <t>教师培训</t>
+        </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -994,26 +913,23 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>平昌县西兴镇人民政府</t>
+          <t>平昌县教育科技局</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>义务教育</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">西兴镇2024年食品药品安全工作实施方案                                            </t>
+          <t>教育督导</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-26</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>87</v>
+          <t>机构队伍</t>
+        </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1027,26 +943,23 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>平昌县西兴镇人民政府</t>
+          <t>平昌县司法局</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>公共法律</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">西兴镇道路管护制度                                            </t>
+          <t>法治宣传教育</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-22</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>91</v>
+          <t>推广法治文化服务</t>
+        </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1060,26 +973,23 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>平昌县龙岗镇人民政府</t>
+          <t>平昌县司法局</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>公共法律</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">龙岗镇人关于开展高龄津贴发放对象年审工作的通知                                            </t>
+          <t>法律援助</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-07-19</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>94</v>
+          <t>法律援助办案人员办案补贴的审核发放</t>
+        </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1093,26 +1003,23 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>平昌县龙岗镇人民政府</t>
+          <t>平昌县司法局</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>公共法律</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">龙岗镇关于艾滋病重点领域综合防治工作实施方案                                            </t>
+          <t>法律查询服务</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024-07-18</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>95</v>
+          <t>法律服务机构、人员信息查询服务</t>
+        </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1126,26 +1033,18 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>平昌县土垭镇人民政府</t>
+          <t>平昌县自然资源和规划局</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>自然资源</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">开展特殊困难老年人探访关爱服务实施方案的通知                                            </t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2024-07-23</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>90</v>
+          <t>调查监测</t>
+        </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1159,26 +1058,18 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>平昌县佛楼镇人民政府</t>
+          <t>平昌县自然资源和规划局</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>自然资源</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">佛楼镇集中开展“四防”安全宣传教育活动工作方案                                            </t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>81</v>
+          <t>生态修复</t>
+        </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1192,26 +1083,18 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>平昌县响滩镇人民政府</t>
+          <t>平昌县自然资源和规划局</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>统计信息</t>
+          <t>自然资源</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">响滩镇2024年二季度蔬菜、瓜果生产情况统计表                                            </t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2024-07-30</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>83</v>
+          <t>耕地保护</t>
+        </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1225,26 +1108,18 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>平昌县驷马镇人民政府</t>
+          <t>平昌县自然资源和规划局</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>统计信息</t>
+          <t>自然资源</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">驷马镇2024年二季度蔬菜、瓜果生产情况统计                                            </t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2024-07-12</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>101</v>
+          <t>地质灾害预防和治理</t>
+        </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1258,26 +1133,18 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>平昌县驷马镇人民政府</t>
+          <t>平昌县综合行政执法局</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>城市综合执法</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">驷马镇安全生产治本攻坚三年行动实施方案(2024-2026年)                                            </t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2024-07-05</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>108</v>
+          <t>行政许可</t>
+        </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1291,26 +1158,18 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>平昌县驷马镇人民政府</t>
+          <t>平昌县财政局</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>财政预决算</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">驷马镇关于切实做好夏季防溺水工作的通知                                            </t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2024-07-05</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>108</v>
+          <t>财政预算</t>
+        </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1324,26 +1183,18 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>平昌县青云镇人民政府</t>
+          <t>平昌县统计局</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>统计领域</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">青云镇关于开展“红色代办队”帮代办服务的实施方案                                            </t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2024-07-25</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
-        <v>88</v>
+          <t>行政处罚信息公示</t>
+        </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1357,26 +1208,18 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>平昌县青云镇人民政府</t>
+          <t>平昌县统计局</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>统计领域</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">青云镇大气污染防治工作方法                                            </t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2024-07-25</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>88</v>
+          <t>统计执法监督</t>
+        </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1390,26 +1233,18 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>平昌县澌岸镇人民政府</t>
+          <t>县公共资源交易服务中心</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>公共资源交易</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">澌岸镇2024年7月困难救助公示表                                            </t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2024-07-26</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>87</v>
+          <t>国有土地使用权出让信息</t>
+        </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1423,26 +1258,18 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>平昌县澌岸镇人民政府</t>
+          <t>平昌县交通运输局</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>交通运输</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">平昌县澌岸镇人民政府2023年部门整体支出绩效评价报告                                            </t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>2024-07-26</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>87</v>
+          <t>行政处罚</t>
+        </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1456,26 +1283,18 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>平昌县元山镇人民政府</t>
+          <t>平昌县交通运输局</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>统计信息</t>
+          <t>交通运输</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">元山镇2024年二季度中药材数据台账                                            </t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>2024-07-29</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>84</v>
+          <t>规划计划</t>
+        </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1489,26 +1308,18 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>平昌县灵山镇人民政府</t>
+          <t>平昌县交通运输局</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>民生保障</t>
+          <t>交通运输</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">灵山镇2024年安全宣传“五进”工作实施方案                                            </t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>2024-07-29</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
-        <v>84</v>
+          <t>建设管理</t>
+        </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1522,26 +1333,18 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>平昌县灵山镇人民政府</t>
+          <t>平昌县应急管理局</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>安全生产</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">平昌县灵山镇便民服务中心管理制度                                            </t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>2024-07-26</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>87</v>
+          <t>行政强制</t>
+        </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1555,26 +1358,18 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>平昌县土兴镇人民政府</t>
+          <t>平昌县应急管理局</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>规划计划</t>
+          <t>救灾领域</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">土兴镇2023年安全生产应急管理工作计划                                            </t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>2023-10-19</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>368</v>
+          <t>备灾管理</t>
+        </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1588,26 +1383,18 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>平昌县三十二梁镇人民政府</t>
+          <t>平昌县应急管理局</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>其他法定信息</t>
+          <t>救灾领域</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">三十二梁旅游景区研学基地拓片区域全面竣工                                            </t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>2024-07-22</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>91</v>
+          <t>灾后救助</t>
+        </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -1621,26 +1408,18 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>平昌县邱家镇人民政府</t>
+          <t>平昌县应急管理局</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>统计信息</t>
+          <t>救灾领域</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">邱家镇2024年二季度经济作物指导性任务表                                            </t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>2024-07-17</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>96</v>
+          <t>灾害救助</t>
+        </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -1652,32 +1431,9 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>平昌县邱家镇人民政府</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>其他法定信息</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">关于对2024年汛期乡村公路水毁安全隐患进行整治的通知                                            </t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>2024-07-30</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>83</v>
-      </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>放管服改革</t>
+          <t>卫生健康</t>
         </is>
       </c>
       <c r="K39" t="n">
@@ -1685,9 +1441,18 @@
       </c>
     </row>
     <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>3.以下位置相邻文章发布时间间隔大于90天</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="n"/>
+      <c r="C40" s="2" t="n"/>
+      <c r="D40" s="2" t="n"/>
+      <c r="E40" s="2" t="n"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>卫生健康</t>
+          <t>价格监测</t>
         </is>
       </c>
       <c r="K40" t="n">
@@ -1695,94 +1460,29 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="inlineStr">
-        <is>
-          <t>2.死链监测：以下单位对应栏目无内容，请上传内容或审核发布</t>
-        </is>
-      </c>
-      <c r="B41" s="2" t="n"/>
-      <c r="C41" s="2" t="n"/>
-      <c r="D41" s="2" t="n"/>
-      <c r="E41" s="2" t="n"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>单位名称</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>领域</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>一级事项</t>
+        </is>
+      </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>价格监测</t>
+          <t>民生保障</t>
         </is>
       </c>
       <c r="K41" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="inlineStr">
-        <is>
-          <t>单位名称</t>
-        </is>
-      </c>
-      <c r="B42" s="2" t="inlineStr">
-        <is>
-          <t>栏目名称</t>
-        </is>
-      </c>
-      <c r="C42" s="2" t="n"/>
-      <c r="D42" s="2" t="n"/>
-      <c r="E42" s="2" t="n"/>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>民生保障</t>
-        </is>
-      </c>
-      <c r="K42" t="n">
         <v>80</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="inlineStr">
-        <is>
-          <t>3.统计信息缺失年份：以下单位缺失对应年份统计信息，请补充</t>
-        </is>
-      </c>
-      <c r="B44" s="2" t="n"/>
-      <c r="C44" s="2" t="n"/>
-      <c r="D44" s="2" t="n"/>
-      <c r="E44" s="2" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="inlineStr">
-        <is>
-          <t>单位名称</t>
-        </is>
-      </c>
-      <c r="B45" s="2" t="inlineStr">
-        <is>
-          <t>缺失年份</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="n"/>
-      <c r="D45" s="2" t="n"/>
-      <c r="E45" s="2" t="n"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>二、政府信息公开年报栏目缺失情况监测</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="2" t="inlineStr">
-        <is>
-          <t>单位名称</t>
-        </is>
-      </c>
-      <c r="B48" s="2" t="inlineStr">
-        <is>
-          <t>缺失年份</t>
-        </is>
-      </c>
-      <c r="C48" s="2" t="n"/>
-      <c r="D48" s="2" t="n"/>
-      <c r="E48" s="2" t="n"/>
     </row>
     <row r="49">
       <c r="J49" s="2" t="inlineStr">
@@ -1792,11 +1492,6 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>三、机构职能页监测</t>
-        </is>
-      </c>
       <c r="J50" t="inlineStr">
         <is>
           <t>1.每个事项的总内容不少于4条</t>
@@ -1804,11 +1499,6 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>1.以下位置未发布，请管理员处理</t>
-        </is>
-      </c>
       <c r="J51" t="inlineStr">
         <is>
           <t>2.最新更新时间不大于90天</t>
@@ -1823,94 +1513,15 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>2.以下位置链接状态错误，请管理员检查</t>
-        </is>
-      </c>
       <c r="J53" t="inlineStr">
         <is>
           <t>注意：除办事服务等不易发布的内容外，其余链接形式的内容应尽量粘贴复制而不是直接跳转，否则机器人无法监测</t>
         </is>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>3.以下单位机关简介中无领导分管政务公开，请对应部门修改</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>县经济和信息化局</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>4.以下单位机关简介中时间表述错误，请对应部门修改</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>四、政府信息政策栏超期情况</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="2" t="inlineStr">
-        <is>
-          <t>单位名称</t>
-        </is>
-      </c>
-      <c r="B60" s="2" t="inlineStr">
-        <is>
-          <t>更新标题</t>
-        </is>
-      </c>
-      <c r="C60" s="2" t="inlineStr">
-        <is>
-          <t>最后更新时间</t>
-        </is>
-      </c>
-      <c r="D60" s="2" t="inlineStr">
-        <is>
-          <t>超期天数</t>
-        </is>
-      </c>
-      <c r="E60" s="2" t="n"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>平昌县医疗保障局</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">平昌县2024年度城乡居民基本医疗保险政策                                            </t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>2023-09-11</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>406</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A50:D50"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>